<commit_message>
Added - Util functoin for delete temp files.
</commit_message>
<xml_diff>
--- a/data/emp_collect.xlsx
+++ b/data/emp_collect.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Cloud_EMS" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="EMS" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Emp_Id</t>
   </si>
@@ -35,6 +35,27 @@
   </si>
   <si>
     <t>Salary</t>
+  </si>
+  <si>
+    <t>David10</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>David11</t>
+  </si>
+  <si>
+    <t>David12</t>
+  </si>
+  <si>
+    <t>David13</t>
+  </si>
+  <si>
+    <t>David14</t>
+  </si>
+  <si>
+    <t>David17</t>
   </si>
 </sst>
 </file>
@@ -70,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="10" customWidth="1"/>
@@ -447,6 +469,144 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>9578821821</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1">
+        <v>40319</v>
+      </c>
+      <c r="H2">
+        <v>50009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>9578821821</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1">
+        <v>40320</v>
+      </c>
+      <c r="H3">
+        <v>50010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>9578821821</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1">
+        <v>40321</v>
+      </c>
+      <c r="H4">
+        <v>50011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>9578821821</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1">
+        <v>40322</v>
+      </c>
+      <c r="H5">
+        <v>50012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>114</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>9578821821</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1">
+        <v>40323</v>
+      </c>
+      <c r="H6">
+        <v>50013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>9578821821</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1">
+        <v>40326</v>
+      </c>
+      <c r="H7">
+        <v>50016</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>